<commit_message>
Forms working, woaah even an excel
</commit_message>
<xml_diff>
--- a/www/files/adventures.xlsx
+++ b/www/files/adventures.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>orderNumber</t>
   </si>
@@ -26,6 +26,9 @@
     <t>date</t>
   </si>
   <si>
+    <t>participantsCount</t>
+  </si>
+  <si>
     <t>department</t>
   </si>
   <si>
@@ -50,7 +53,7 @@
     <t>2024-08-01 10:00:00</t>
   </si>
   <si>
-    <t>Beavers</t>
+    <t>Veverky</t>
   </si>
   <si>
     <t>Provider A</t>
@@ -68,7 +71,7 @@
     <t>2024-08-15 12:00:00</t>
   </si>
   <si>
-    <t>Cubs</t>
+    <t>Bobři</t>
   </si>
   <si>
     <t>Provider B</t>
@@ -86,7 +89,7 @@
     <t>2024-09-05 14:00:00</t>
   </si>
   <si>
-    <t>Scouts</t>
+    <t>Křečci</t>
   </si>
   <si>
     <t>Provider C</t>
@@ -432,7 +435,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,7 +443,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,18 +468,21 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
         <v>11</v>
       </c>
       <c r="E2" t="s">
@@ -485,25 +491,28 @@
       <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2">
         <v>500.0</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>450.0</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
         <v>17</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -511,22 +520,25 @@
       <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
         <v>300.0</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
         <v>23</v>
+      </c>
+      <c r="D4">
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -534,10 +546,13 @@
       <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4">
         <v>600.0</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>600.0</v>
       </c>
     </row>

</xml_diff>